<commit_message>
325 Sign APK files
</commit_message>
<xml_diff>
--- a/Project Documents/Give and Take App Accounts.xlsx
+++ b/Project Documents/Give and Take App Accounts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Infrastructure</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,11 +584,17 @@
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3">

</xml_diff>